<commit_message>
Added XLSX to SearchMySQLInstances
</commit_message>
<xml_diff>
--- a/resources/templates/template_generic.xlsx
+++ b/resources/templates/template_generic.xlsx
@@ -126,11 +126,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AW1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BD1" activeCellId="0" sqref="BD1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="22.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>